<commit_message>
remove twice diff test, set start date to 1986
</commit_message>
<xml_diff>
--- a/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/SUR2006-02-28-2020-02-29.xlsx
+++ b/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/SUR2006-02-28-2020-02-29.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>LF_C</t>
-  </si>
-  <si>
-    <t>A_C</t>
+    <t>C_A</t>
   </si>
   <si>
     <t>FFR_A</t>
   </si>
   <si>
-    <t>C_A</t>
+    <t>LF_FFR</t>
+  </si>
+  <si>
+    <t>A_FFR</t>
   </si>
   <si>
     <t>params</t>
@@ -414,16 +414,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>-78.29729548487525</v>
+        <v>0.0674807823212608</v>
       </c>
       <c r="C2">
-        <v>10.19294504512097</v>
+        <v>-2.892896467187215</v>
       </c>
       <c r="D2">
-        <v>-1.821719970535869</v>
+        <v>2.154824654788232</v>
       </c>
       <c r="E2">
-        <v>0.08755023134145418</v>
+        <v>-0.1938798303935576</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -431,13 +431,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1.288281721301132E-06</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1.849409514420586E-12</v>
+        <v>1.71112393143602E-08</v>
       </c>
       <c r="E3">
         <v>0</v>

</xml_diff>